<commit_message>
modified test data file
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EclipseWorkspace\LumaProject01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F332B8-03DA-488D-9811-0884AAAB0A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D9197B-1216-4BD2-ADF9-93B6F732D341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{682B5F53-B4C6-4718-8BF6-8FCF18E56293}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Sup</t>
+    <t>Supriya</t>
+  </si>
+  <si>
+    <t>Sup@123</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -419,10 +422,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{2537FAEF-5022-452B-8C17-89EAC2585106}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>